<commit_message>
Updated Data: 1) DRI data, 2) Update few TAZ areaTypes to "Transitional", 3) add review density
</commit_message>
<xml_diff>
--- a/Input/base_data/gen max densitys by area type.xlsx
+++ b/Input/base_data/gen max densitys by area type.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Models\StateWide\TSM_Legacy\FLUAM\Input\base_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9F0FB66-9F89-402B-8DDB-607922943FD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0255C3D6-7F93-4EB9-B4F9-A954596DE8FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="345" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B60FA2BC-C576-4A65-A82B-BC82E30E5552}"/>
+    <workbookView xWindow="30600" yWindow="1305" windowWidth="25830" windowHeight="13635" activeTab="1" xr2:uid="{B60FA2BC-C576-4A65-A82B-BC82E30E5552}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="reformat" sheetId="2" r:id="rId2"/>
-    <sheet name="reformat2" sheetId="3" r:id="rId3"/>
+    <sheet name="reformat2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="35">
   <si>
     <t>Miami Dade</t>
   </si>
@@ -122,28 +121,7 @@
     <t>All Others</t>
   </si>
   <si>
-    <t xml:space="preserve"> growthCenter</t>
-  </si>
-  <si>
     <t>County</t>
-  </si>
-  <si>
-    <t>HH.U</t>
-  </si>
-  <si>
-    <t>EMP.U</t>
-  </si>
-  <si>
-    <t>HH.T</t>
-  </si>
-  <si>
-    <t>EMP.T</t>
-  </si>
-  <si>
-    <t>HH.R</t>
-  </si>
-  <si>
-    <t>EMP.R</t>
   </si>
   <si>
     <t>growthCenter</t>
@@ -165,17 +143,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -301,9 +272,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,634 +983,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5512CAEC-0BD7-4FA7-84EA-55AE29834AFA}">
-  <dimension ref="A1:H24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>50</v>
-      </c>
-      <c r="D2" s="3">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <v>25</v>
-      </c>
-      <c r="F2" s="6">
-        <v>50</v>
-      </c>
-      <c r="G2" s="8">
-        <v>5</v>
-      </c>
-      <c r="H2" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <v>15</v>
-      </c>
-      <c r="F3" s="6">
-        <v>30</v>
-      </c>
-      <c r="G3" s="8">
-        <v>5</v>
-      </c>
-      <c r="H3" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>50</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-      <c r="F4" s="6">
-        <v>30</v>
-      </c>
-      <c r="G4" s="8">
-        <v>5</v>
-      </c>
-      <c r="H4" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3">
-        <v>35</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6">
-        <v>25</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>56</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3">
-        <v>35</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>43</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3">
-        <v>35</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6">
-        <v>25</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3">
-        <v>35</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="6">
-        <v>25</v>
-      </c>
-      <c r="G9" s="8">
-        <v>5</v>
-      </c>
-      <c r="H9" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>55</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3">
-        <v>35</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10" s="6">
-        <v>25</v>
-      </c>
-      <c r="G10" s="8">
-        <v>5</v>
-      </c>
-      <c r="H10" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3">
-        <v>35</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" s="6">
-        <v>25</v>
-      </c>
-      <c r="G11" s="8">
-        <v>5</v>
-      </c>
-      <c r="H11" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>29</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3">
-        <v>50</v>
-      </c>
-      <c r="E12">
-        <v>15</v>
-      </c>
-      <c r="F12" s="6">
-        <v>30</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>52</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3">
-        <v>50</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="F13" s="6">
-        <v>30</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>51</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="2">
-        <v>25</v>
-      </c>
-      <c r="D14" s="3">
-        <v>50</v>
-      </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
-      <c r="F14" s="6">
-        <v>30</v>
-      </c>
-      <c r="G14">
-        <v>5</v>
-      </c>
-      <c r="H14" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>53</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="2">
-        <v>25</v>
-      </c>
-      <c r="D15" s="3">
-        <v>50</v>
-      </c>
-      <c r="E15">
-        <v>15</v>
-      </c>
-      <c r="F15" s="6">
-        <v>30</v>
-      </c>
-      <c r="G15">
-        <v>5</v>
-      </c>
-      <c r="H15" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>49</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="2">
-        <v>25</v>
-      </c>
-      <c r="D16" s="3">
-        <v>50</v>
-      </c>
-      <c r="E16">
-        <v>15</v>
-      </c>
-      <c r="F16" s="6">
-        <v>30</v>
-      </c>
-      <c r="G16">
-        <v>5</v>
-      </c>
-      <c r="H16" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>48</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="2">
-        <v>25</v>
-      </c>
-      <c r="D17" s="3">
-        <v>50</v>
-      </c>
-      <c r="E17">
-        <v>15</v>
-      </c>
-      <c r="F17" s="6">
-        <v>30</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>59</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="2">
-        <v>25</v>
-      </c>
-      <c r="D18" s="3">
-        <v>50</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
-      <c r="F18" s="6">
-        <v>30</v>
-      </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>64</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="2">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3">
-        <v>50</v>
-      </c>
-      <c r="E19">
-        <v>15</v>
-      </c>
-      <c r="F19" s="6">
-        <v>30</v>
-      </c>
-      <c r="G19">
-        <v>5</v>
-      </c>
-      <c r="H19" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2">
-        <v>20</v>
-      </c>
-      <c r="D20" s="3">
-        <v>35</v>
-      </c>
-      <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20" s="6">
-        <v>25</v>
-      </c>
-      <c r="G20" s="8">
-        <v>5</v>
-      </c>
-      <c r="H20" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>11</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2">
-        <v>20</v>
-      </c>
-      <c r="D21" s="3">
-        <v>35</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21" s="6">
-        <v>25</v>
-      </c>
-      <c r="G21" s="8">
-        <v>5</v>
-      </c>
-      <c r="H21" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>57</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="2">
-        <v>15</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="G22" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>37</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2">
-        <v>15</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="G23" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="2">
-        <v>15</v>
-      </c>
-      <c r="D24" s="3">
-        <v>25</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24" s="6">
-        <v>15</v>
-      </c>
-      <c r="G24" s="8">
-        <v>5</v>
-      </c>
-      <c r="H24" s="9">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4577C3-64E7-4C96-B8D5-57663389783C}">
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,22 +997,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>